<commit_message>
Pulled BoM.xlsx, also changed pull ups to 0805
</commit_message>
<xml_diff>
--- a/BoM.xlsx
+++ b/BoM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\GitHub\PCB-Workshop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurence\Documents\GitHub\PCB-Workshop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="56">
   <si>
     <t>Schematic Reference</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t>http://www.ragworm.eu</t>
+  </si>
+  <si>
+    <t>R7 R8</t>
+  </si>
+  <si>
+    <t>10K</t>
   </si>
 </sst>
 </file>
@@ -712,26 +718,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="B2:M29"/>
+  <dimension ref="B2:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="151.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="151.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>39</v>
       </c>
@@ -742,24 +748,24 @@
         <v>46</v>
       </c>
       <c r="E2" s="7">
-        <f>SUM(I6:I19)</f>
-        <v>102.089</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
+        <f>SUM(I6:I20)</f>
+        <v>102.26900000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D3" s="6" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="7">
         <f>E2/C2</f>
-        <v>5.1044499999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>5.1134500000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="6"/>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>0</v>
       </c>
@@ -791,7 +797,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
         <v>6</v>
       </c>
@@ -826,7 +832,7 @@
       </c>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
         <v>7</v>
       </c>
@@ -846,11 +852,11 @@
         <v>50</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" ref="H7:H17" si="0">MAX(C7*$C$2,G7)</f>
+        <f t="shared" ref="H7:H18" si="0">MAX(C7*$C$2,G7)</f>
         <v>50</v>
       </c>
       <c r="I7" s="10">
-        <f t="shared" ref="I7:I19" si="1">F7*H7</f>
+        <f t="shared" ref="I7:I20" si="1">F7*H7</f>
         <v>0.42500000000000004</v>
       </c>
       <c r="J7" s="8" t="s">
@@ -861,7 +867,7 @@
       </c>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>11</v>
       </c>
@@ -896,7 +902,7 @@
       </c>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
@@ -931,21 +937,21 @@
       </c>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C10" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>16</v>
+        <v>55</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F10" s="10">
-        <v>0.03</v>
+        <v>1.8E-3</v>
       </c>
       <c r="G10" s="8">
         <v>100</v>
@@ -956,32 +962,31 @@
       </c>
       <c r="I10" s="10">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>0.18</v>
       </c>
       <c r="J10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="20" t="s">
-        <v>40</v>
+      <c r="K10" s="20">
+        <v>2447553</v>
       </c>
       <c r="L10" s="5"/>
-      <c r="M10"/>
-    </row>
-    <row r="11" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="10">
-        <v>7.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
       <c r="G11" s="8">
         <v>100</v>
@@ -992,104 +997,104 @@
       </c>
       <c r="I11" s="10">
         <f t="shared" si="1"/>
-        <v>0.70000000000000007</v>
+        <v>3</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>35</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L11" s="5"/>
       <c r="M11"/>
     </row>
-    <row r="12" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F12" s="10">
-        <v>3.1199999999999999E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G12" s="8">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H12" s="8">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="I12" s="10">
         <f t="shared" si="1"/>
-        <v>1.248</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K12" s="20">
-        <v>8735654</v>
+      <c r="K12" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="L12" s="5"/>
       <c r="M12"/>
     </row>
-    <row r="13" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C13" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F13" s="10">
-        <v>5.4100000000000002E-2</v>
+        <v>3.1199999999999999E-2</v>
       </c>
       <c r="G13" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H13" s="8">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="I13" s="10">
         <f t="shared" si="1"/>
-        <v>1.0820000000000001</v>
+        <v>1.248</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>35</v>
       </c>
       <c r="K13" s="20">
-        <v>1226372</v>
+        <v>8735654</v>
       </c>
       <c r="L13" s="5"/>
       <c r="M13"/>
     </row>
-    <row r="14" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="10">
-        <v>5.62E-2</v>
+        <v>5.4100000000000002E-2</v>
       </c>
       <c r="G14" s="8">
         <v>1</v>
@@ -1100,32 +1105,32 @@
       </c>
       <c r="I14" s="10">
         <f t="shared" si="1"/>
-        <v>1.1240000000000001</v>
+        <v>1.0820000000000001</v>
       </c>
       <c r="J14" s="8" t="s">
         <v>35</v>
       </c>
       <c r="K14" s="20">
-        <v>2099221</v>
+        <v>1226372</v>
       </c>
       <c r="L14" s="5"/>
       <c r="M14"/>
     </row>
-    <row r="15" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="10">
-        <v>1.05</v>
+        <v>5.62E-2</v>
       </c>
       <c r="G15" s="8">
         <v>1</v>
@@ -1136,34 +1141,35 @@
       </c>
       <c r="I15" s="10">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>1.1240000000000001</v>
       </c>
       <c r="J15" s="8" t="s">
         <v>35</v>
       </c>
       <c r="K15" s="20">
-        <v>1455164</v>
+        <v>2099221</v>
       </c>
       <c r="L15" s="5"/>
-    </row>
-    <row r="16" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F16" s="10">
-        <v>0.71699999999999997</v>
+        <v>1.05</v>
       </c>
       <c r="G16" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H16" s="8">
         <f t="shared" si="0"/>
@@ -1171,31 +1177,31 @@
       </c>
       <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>14.34</v>
+        <v>21</v>
       </c>
       <c r="J16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="22">
-        <v>2080524</v>
+      <c r="K16" s="20">
+        <v>1455164</v>
       </c>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C17" s="8">
         <v>1</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>43</v>
+      <c r="D17" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="F17" s="10">
-        <v>0.31900000000000001</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="G17" s="8">
         <v>10</v>
@@ -1206,87 +1212,111 @@
       </c>
       <c r="I17" s="10">
         <f t="shared" si="1"/>
-        <v>6.38</v>
+        <v>14.34</v>
       </c>
       <c r="J17" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="22">
+        <v>2080524</v>
+      </c>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="G18" s="8">
+        <v>10</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="1"/>
+        <v>6.38</v>
+      </c>
+      <c r="J18" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" s="20">
         <v>2112367</v>
       </c>
-      <c r="L17" s="5"/>
-    </row>
-    <row r="18" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="14" t="s">
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C19" s="8">
         <v>2</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="8">
+      <c r="F19" s="10"/>
+      <c r="G19" s="8">
         <v>100</v>
       </c>
-      <c r="H18" s="8">
-        <f>MAX(C18*$C$2,G18)</f>
+      <c r="H19" s="8">
+        <f>MAX(C19*$C$2,G19)</f>
         <v>100</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I19" s="10">
         <v>2.15</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K19" s="20" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="15" t="s">
+    <row r="20" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="16">
+      <c r="C20" s="16">
         <v>1</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="18">
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="18">
         <v>2.5</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16">
-        <f>MAX(C19*$C$2,G19)</f>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16">
+        <f>MAX(C20*$C$2,G20)</f>
         <v>20</v>
       </c>
-      <c r="I19" s="18">
+      <c r="I20" s="18">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J20" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="K19" s="23" t="s">
+      <c r="K20" s="23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1297,7 +1327,7 @@
       <c r="I21" s="2"/>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1308,7 +1338,7 @@
       <c r="I22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1319,7 +1349,7 @@
       <c r="I23" s="2"/>
       <c r="K23" s="2"/>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1330,7 +1360,7 @@
       <c r="I24" s="2"/>
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1341,7 +1371,7 @@
       <c r="I25" s="2"/>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1352,7 +1382,7 @@
       <c r="I26" s="2"/>
       <c r="K26" s="2"/>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1363,7 +1393,7 @@
       <c r="I27" s="2"/>
       <c r="K27" s="2"/>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1374,7 +1404,7 @@
       <c r="I28" s="2"/>
       <c r="K28" s="2"/>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1385,27 +1415,39 @@
       <c r="I29" s="2"/>
       <c r="K29" s="2"/>
     </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="K30" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K6" r:id="rId1" tooltip="2447623" display="http://onecall.farnell.com/multicomp/mcwr08x2201ftl/res-thick-film-2-2kohm-1-0-125w/dp/2447623"/>
     <hyperlink ref="K7" r:id="rId2" tooltip="2138823" display="http://onecall.farnell.com/vishay-draloric/crcw080568r0fkea/resistor-0805-68r-1/dp/2138823"/>
     <hyperlink ref="K8" r:id="rId3" tooltip="9234098" display="http://onecall.farnell.com/yageo-phycomp/rc0805jr-074k7l/resistor-rc11-0805-4k7/dp/9234098"/>
     <hyperlink ref="K9" r:id="rId4" tooltip="2447638" display="http://onecall.farnell.com/multicomp/mcwr08x3300ftl/res-thick-film-330-ohm-1-0-125w/dp/2447638"/>
-    <hyperlink ref="K10" r:id="rId5" tooltip="CA06400" display="http://onecall.farnell.com/multicomp/mcca000268/mlcc-0805-y5v-6-3v-10uf/dp/CA06400"/>
-    <hyperlink ref="K11" r:id="rId6" tooltip="CA06475" display="http://onecall.farnell.com/multicomp/mcca000387/mlcc-0805-y5v-50v-100nf/dp/CA06475"/>
-    <hyperlink ref="K12" r:id="rId7" tooltip="8735654" display="http://onecall.farnell.com/nxp/bzx384-c3v6/diode-zener-3-6v-5-sod-323/dp/8735654"/>
-    <hyperlink ref="K14" r:id="rId8" tooltip="2099221" display="http://onecall.farnell.com/kingbright/kpt-1608ec/led-0603-red-15mcd-625nm/dp/2099221"/>
-    <hyperlink ref="K13" r:id="rId9" tooltip="1226372" display="http://onecall.farnell.com/osram/lgq971/led-green-10mcd-570nm-smd/dp/1226372"/>
-    <hyperlink ref="K15" r:id="rId10" tooltip="1455164" display="http://onecall.farnell.com/atmel/attiny85-20su/mcu-8bit-attiny-20mhz-soic-8/dp/1455164"/>
-    <hyperlink ref="K17" r:id="rId11" tooltip="2112367" display="http://onecall.farnell.com/fci/10033526-n3212mlf/mini-usb-2-0-type-b-receptacle/dp/2112367"/>
-    <hyperlink ref="K18" r:id="rId12"/>
-    <hyperlink ref="K16" r:id="rId13" tooltip="2080524" display="http://onecall.farnell.com/microchip/mcp9808t-e-mc/temp-sensor-i2c-20-to-100-deg/dp/2080524"/>
-    <hyperlink ref="K19" r:id="rId14"/>
+    <hyperlink ref="K11" r:id="rId5" tooltip="CA06400" display="http://onecall.farnell.com/multicomp/mcca000268/mlcc-0805-y5v-6-3v-10uf/dp/CA06400"/>
+    <hyperlink ref="K12" r:id="rId6" tooltip="CA06475" display="http://onecall.farnell.com/multicomp/mcca000387/mlcc-0805-y5v-50v-100nf/dp/CA06475"/>
+    <hyperlink ref="K13" r:id="rId7" tooltip="8735654" display="http://onecall.farnell.com/nxp/bzx384-c3v6/diode-zener-3-6v-5-sod-323/dp/8735654"/>
+    <hyperlink ref="K15" r:id="rId8" tooltip="2099221" display="http://onecall.farnell.com/kingbright/kpt-1608ec/led-0603-red-15mcd-625nm/dp/2099221"/>
+    <hyperlink ref="K14" r:id="rId9" tooltip="1226372" display="http://onecall.farnell.com/osram/lgq971/led-green-10mcd-570nm-smd/dp/1226372"/>
+    <hyperlink ref="K16" r:id="rId10" tooltip="1455164" display="http://onecall.farnell.com/atmel/attiny85-20su/mcu-8bit-attiny-20mhz-soic-8/dp/1455164"/>
+    <hyperlink ref="K18" r:id="rId11" tooltip="2112367" display="http://onecall.farnell.com/fci/10033526-n3212mlf/mini-usb-2-0-type-b-receptacle/dp/2112367"/>
+    <hyperlink ref="K19" r:id="rId12"/>
+    <hyperlink ref="K17" r:id="rId13" tooltip="2080524" display="http://onecall.farnell.com/microchip/mcp9808t-e-mc/temp-sensor-i2c-20-to-100-deg/dp/2080524"/>
+    <hyperlink ref="K20" r:id="rId14"/>
+    <hyperlink ref="K10" r:id="rId15" display="http://onecall.farnell.com/multicomp/mcwr08x1002ftl/res-thick-film-10kohm-1-0-125w/dp/2447553"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
   <ignoredErrors>
-    <ignoredError sqref="E6:E11" numberStoredAsText="1"/>
+    <ignoredError sqref="E11:E12 E6:E9" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>